<commit_message>
data updated till 10Jan 10AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -42,10 +42,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -65,7 +65,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -78,10 +78,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -93,10 +94,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -108,9 +126,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,9 +141,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,6 +158,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -146,6 +185,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,55 +200,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,187 +229,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,15 +420,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,6 +447,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -467,6 +467,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,44 +520,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,131 +546,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -681,9 +681,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1008,13 +1005,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.2857142857143" style="1"/>
     <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
@@ -1036,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:14">
       <c r="A2" s="3">
         <v>44185</v>
       </c>
@@ -1046,8 +1043,14 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="M2" s="1">
+        <v>6918</v>
+      </c>
+      <c r="N2" s="1">
+        <v>3100</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>44192</v>
       </c>
@@ -1056,15 +1059,40 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>-3098</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3">
+        <v>43840</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3820</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
+        <f>SUM(M2:M3)</f>
+        <v>3820</v>
+      </c>
+      <c r="N4" s="1">
+        <f>SUM(N2:N3)</f>
+        <v>6920</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <f>SUM(B2:B22)</f>
-        <v>3350</v>
+        <v>7170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updated till 11 Jan 9 PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -42,10 +42,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -64,6 +64,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -72,9 +87,63 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -86,92 +155,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,6 +170,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -192,17 +185,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,187 +229,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,11 +423,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -451,7 +481,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,23 +504,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,27 +520,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,130 +543,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1005,13 +1005,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="M2" sqref="M2:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.2857142857143" style="1"/>
     <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
@@ -1033,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>44185</v>
       </c>
@@ -1043,14 +1043,8 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1">
-        <v>6918</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3100</v>
-      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>44192</v>
       </c>
@@ -1060,14 +1054,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="1">
-        <v>-3098</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3820</v>
-      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>43840</v>
       </c>
@@ -1076,14 +1064,6 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="M4" s="1">
-        <f>SUM(M2:M3)</f>
-        <v>3820</v>
-      </c>
-      <c r="N4" s="1">
-        <f>SUM(N2:N3)</f>
-        <v>6920</v>
       </c>
     </row>
     <row r="23" spans="1:2">

</xml_diff>

<commit_message>
data updated till 21 Jan 9AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -45,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -64,6 +64,66 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -76,91 +136,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,8 +165,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -183,7 +197,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,21 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,6 +232,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -244,7 +346,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,163 +376,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,41 +429,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,6 +465,50 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -512,164 +523,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1090,13 +1090,27 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>44216</v>
+      </c>
+      <c r="B6" s="1">
+        <v>253</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>7933</v>
+        <v>8186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 25 Jan 9PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -46,9 +46,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -68,14 +68,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -88,11 +143,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -104,54 +173,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,7 +190,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,22 +198,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -197,15 +205,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,37 +232,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,19 +388,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,121 +412,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,15 +423,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,30 +437,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,7 +460,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,6 +496,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,148 +528,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1104,13 +1104,24 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>44221</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3470</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>8186</v>
+        <v>11656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 29 Jan 7PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -46,9 +46,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -83,7 +83,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,17 +91,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -113,9 +105,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,39 +120,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -174,14 +166,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -189,6 +173,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -198,14 +197,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,187 +232,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,17 +426,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,11 +465,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,15 +515,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -499,44 +523,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,130 +546,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1115,13 +1115,24 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>44224</v>
+      </c>
+      <c r="B8" s="1">
+        <v>793</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>11656</v>
+        <v>12449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 2Feb 11AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -45,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -83,30 +83,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,38 +104,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,23 +168,29 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,15 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,187 +232,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,30 +423,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -465,6 +441,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -476,15 +472,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,11 +502,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,15 +528,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,130 +546,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1126,13 +1126,24 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>44229</v>
+      </c>
+      <c r="B9" s="1">
+        <v>16317</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>12449</v>
+        <v>28766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 5Feb 3AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -45,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -75,22 +75,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,14 +112,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -121,17 +121,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,22 +165,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -167,9 +173,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,35 +206,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,187 +232,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,6 +423,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -450,13 +461,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,30 +501,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -523,20 +514,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -549,127 +549,127 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1137,13 +1137,27 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
+        <v>44231</v>
+      </c>
+      <c r="B10" s="1">
+        <v>253</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>28766</v>
+        <v>29019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 7Feb 1PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Connectivity</t>
   </si>
   <si>
+    <t>Jio phone X cost refund scheme</t>
+  </si>
+  <si>
     <t>Total:</t>
   </si>
 </sst>
@@ -45,9 +48,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -67,6 +70,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -75,22 +101,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,7 +139,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,46 +153,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,17 +169,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,29 +194,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,187 +235,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,13 +429,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -448,30 +455,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,6 +483,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -514,29 +526,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,130 +549,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1017,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1115,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>44224</v>
       </c>
@@ -1124,6 +1127,9 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1151,13 +1157,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
+        <v>44233</v>
+      </c>
+      <c r="B11" s="1">
+        <v>395</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="3"/>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>29019</v>
+        <v>29414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 14Feb 8PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Connectivity</t>
   </si>
   <si>
+    <t>Sim refund</t>
+  </si>
+  <si>
     <t>Jio phone X cost refund scheme</t>
   </si>
   <si>
@@ -48,10 +51,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -70,38 +73,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,25 +179,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,22 +195,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -179,29 +205,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,181 +238,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,31 +433,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -470,15 +458,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,6 +482,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -511,27 +529,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -549,130 +552,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1017,7 +1020,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1057,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3">
         <v>44192</v>
       </c>
@@ -1067,8 +1070,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="3">
         <v>43840</v>
       </c>
@@ -1077,6 +1083,9 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1107,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="3">
         <v>44221</v>
       </c>
@@ -1116,6 +1125,9 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1129,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1168,19 +1180,44 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3">
+        <v>44235</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3770</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="3"/>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>44238</v>
+      </c>
+      <c r="B13" s="1">
+        <v>253</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>29414</v>
+        <v>33437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 16Feb 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -51,9 +51,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -74,19 +74,49 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -95,6 +125,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -103,30 +179,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,83 +216,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -238,187 +238,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,6 +429,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -443,6 +458,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,17 +506,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -505,36 +529,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,130 +552,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1211,13 +1211,24 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>44242</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2811</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>33437</v>
+        <v>36248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 18Feb 10AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -52,8 +52,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -73,38 +73,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,47 +129,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -171,6 +151,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -182,38 +214,6 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -238,25 +238,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,157 +406,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,17 +432,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -458,6 +482,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,50 +515,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,130 +552,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1211,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="3">
         <v>44242</v>
       </c>
@@ -1220,6 +1220,9 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2">

</xml_diff>

<commit_message>
data till 24Feb 8PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -51,10 +51,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -70,6 +70,105 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -81,17 +180,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -105,92 +196,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,20 +212,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,6 +238,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -250,7 +310,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,19 +334,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,13 +346,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,121 +412,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,15 +429,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,17 +447,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,7 +475,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,23 +509,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,130 +552,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1225,13 +1225,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
+        <v>44251</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4690</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>36248</v>
+        <v>40938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 28Feb 10 PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -51,10 +51,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -74,21 +74,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,14 +112,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -126,26 +126,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -157,6 +142,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -166,7 +158,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,7 +174,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,8 +209,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,13 +238,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,31 +400,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,133 +418,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,6 +429,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -449,24 +464,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,28 +482,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,20 +514,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -552,130 +552,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1225,7 +1225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="3">
         <v>44251</v>
       </c>
@@ -1234,6 +1234,9 @@
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2">

</xml_diff>

<commit_message>
data till 2 Mar 10AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Jio phone X cost refund scheme</t>
   </si>
   <si>
+    <t>GST reimbursement</t>
+  </si>
+  <si>
     <t>Total:</t>
   </si>
 </sst>
@@ -52,9 +55,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -81,6 +84,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -89,14 +122,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,15 +145,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,76 +167,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,187 +241,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,17 +435,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -462,31 +494,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,21 +514,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,130 +555,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,7 +1023,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1239,13 +1242,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>44257</v>
+      </c>
+      <c r="B16" s="1">
+        <v>37838</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="5">
         <f>SUM(B2:B22)</f>
-        <v>40938</v>
+        <v>78776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till Mar 3AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -55,9 +55,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -76,6 +76,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,16 +114,48 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -105,55 +167,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,19 +182,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,28 +214,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,31 +235,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDD56E2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,151 +403,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,6 +438,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -455,41 +476,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,6 +504,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -532,12 +527,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -555,134 +561,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -698,7 +704,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -754,6 +763,11 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="00DD56E2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1023,7 +1037,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1147,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="3">
         <v>44229</v>
       </c>
@@ -1157,6 +1171,7 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3">
@@ -1256,13 +1271,25 @@
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3">
+        <v>44257</v>
+      </c>
+      <c r="B17" s="1">
+        <v>15247</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <f>SUM(B2:B22)</f>
-        <v>78776</v>
+        <v>94023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 4 Mar 3AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
     <t>GST reimbursement</t>
   </si>
   <si>
+    <t>Sim refund??</t>
+  </si>
+  <si>
     <t>Total:</t>
   </si>
 </sst>
@@ -54,10 +57,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -76,15 +79,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -93,7 +149,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -101,28 +172,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,16 +185,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,60 +194,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,187 +250,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,6 +441,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -452,30 +479,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,8 +501,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,7 +511,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -561,130 +564,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1037,7 +1040,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1283,13 +1286,39 @@
       </c>
       <c r="D17" s="5"/>
     </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3">
+        <v>44258</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4950</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3">
+        <v>44258</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8183</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="6">
         <f>SUM(B2:B22)</f>
-        <v>94023</v>
+        <v>107156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 9Mar 11AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -46,7 +46,13 @@
     <t>Jio phone X cost refund scheme</t>
   </si>
   <si>
+    <t>Commission for Jan2021 Vendor ledger</t>
+  </si>
+  <si>
     <t>GST reimbursement</t>
+  </si>
+  <si>
+    <t>Commission for Feb2021 Vendor ledger</t>
   </si>
   <si>
     <t>Sim refund??</t>
@@ -57,10 +63,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -76,6 +82,97 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -87,123 +184,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,13 +256,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,19 +328,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,25 +346,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,115 +382,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,35 +452,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,15 +476,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -514,6 +487,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,6 +518,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -546,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -564,130 +570,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1045,7 +1051,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1077,7 +1083,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>123417</v>
+        <v>133240</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1188,7 +1194,9 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5">
@@ -1285,7 +1293,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1298,7 +1306,9 @@
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5">
@@ -1311,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1324,7 +1334,9 @@
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5">
@@ -1338,8 +1350,17 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5">
+        <v>44263</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9823</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
data till 22Mar 10 PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -63,8 +63,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -85,6 +85,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -92,23 +123,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,38 +141,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,6 +154,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -170,23 +193,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,36 +223,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,187 +256,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,28 +450,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,30 +499,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -547,20 +521,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -570,130 +570,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1046,17 +1046,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.2857142857143" style="1"/>
+    <col min="1" max="1" width="10.4285714285714" style="1"/>
     <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.4285714285714" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>133240</v>
+        <v>134417</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1361,6 +1361,20 @@
         <v>7</v>
       </c>
       <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5">
+        <v>44271</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1177</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
data till 25 Mar 7AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Commission for Jan2021 Vendor ledger</t>
   </si>
   <si>
-    <t>GST reimbursement</t>
+    <t>GST reimbursement for Dec2020 &amp; Jan 2021</t>
   </si>
   <si>
     <t>Commission for Feb2021 Vendor ledger</t>
@@ -57,15 +57,18 @@
   <si>
     <t>Sim refund??</t>
   </si>
+  <si>
+    <t>GST reimbursement for Feb 2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -85,6 +88,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -93,6 +103,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -102,9 +142,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,68 +181,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,13 +202,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -213,15 +225,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -256,25 +259,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,84 +421,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -376,67 +439,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,26 +453,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,6 +489,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -516,8 +521,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,11 +544,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,148 +555,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1046,12 +1049,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1083,7 +1086,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>134417</v>
+        <v>175867</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1374,6 +1377,34 @@
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5">
+        <v>44278</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4590</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5">
+        <v>44280</v>
+      </c>
+      <c r="B25" s="1">
+        <v>36860</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 5 April 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Commission for Feb2021 Vendor ledger</t>
   </si>
   <si>
-    <t>Sim refund??</t>
-  </si>
-  <si>
     <t>GST reimbursement for Feb 2021</t>
   </si>
 </sst>
@@ -66,10 +63,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -89,12 +86,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -104,47 +108,56 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,36 +178,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -202,31 +185,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,19 +256,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,13 +418,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,145 +436,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,41 +447,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -527,6 +489,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -550,20 +536,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,130 +570,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,12 +1046,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1086,7 +1083,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>175867</v>
+        <v>181037</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1324,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1404,7 +1401,21 @@
         <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5">
+        <v>44288</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5170</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 8Apr 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -57,16 +57,19 @@
   <si>
     <t>GST reimbursement for Feb 2021</t>
   </si>
+  <si>
+    <t>Commission for Mar2021 Vendor ledger</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -86,37 +89,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,26 +126,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,6 +150,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -185,6 +188,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -192,38 +225,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,79 +259,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,103 +433,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,6 +450,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,30 +527,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -536,31 +550,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,127 +576,127 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1046,12 +1049,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1083,7 +1086,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>181037</v>
+        <v>197842</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1416,6 +1419,20 @@
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5">
+        <v>44294</v>
+      </c>
+      <c r="B27" s="1">
+        <v>16805</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 14 Apr 10AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -66,8 +66,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -89,22 +89,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,60 +165,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -188,45 +181,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,6 +259,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,37 +325,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,133 +421,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,13 +453,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,21 +507,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -550,12 +539,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -576,127 +576,127 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1054,7 +1054,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
data till 19Apr 8PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -89,14 +89,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,39 +151,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,13 +180,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -165,61 +188,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,187 +259,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,17 +453,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,39 +512,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -531,6 +527,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -539,23 +550,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -573,130 +573,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,12 +1049,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>197842</v>
+        <v>211717</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1433,6 +1433,28 @@
       </c>
       <c r="D27" s="7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>44301</v>
+      </c>
+      <c r="B28" s="1">
+        <v>11290</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>44302</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2585</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 21Apr 9PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Commission for Mar2021 Vendor ledger</t>
+  </si>
+  <si>
+    <t>GST reimbursement for Mar 2021</t>
   </si>
 </sst>
 </file>
@@ -66,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,13 +88,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,72 +99,64 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,7 +169,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -189,12 +177,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -212,21 +214,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,187 +262,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,26 +461,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,6 +491,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,20 +542,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,130 +576,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,12 +1052,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1086,7 +1089,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>211717</v>
+        <v>266675</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1455,6 +1458,34 @@
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5">
+        <v>44307</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5390</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5">
+        <v>44307</v>
+      </c>
+      <c r="B31" s="1">
+        <v>49568</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 4Apr 10AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -69,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -88,6 +88,120 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -99,137 +213,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,13 +262,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,55 +334,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,54 +424,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -400,49 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,6 +453,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -480,30 +506,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -515,6 +517,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,31 +553,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -576,130 +576,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1052,12 +1052,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>266675</v>
+        <v>270875</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1486,6 +1486,20 @@
       </c>
       <c r="D31" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5">
+        <v>44319</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4200</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 13 May 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>GST reimbursement for Mar 2021</t>
+  </si>
+  <si>
+    <t>Commission for Apr2021 Vendor ledger</t>
   </si>
 </sst>
 </file>
@@ -69,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -92,22 +95,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,15 +141,38 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,67 +193,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -213,23 +201,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,13 +265,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +391,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,157 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,13 +459,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,45 +499,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -548,6 +516,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -558,15 +561,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -576,130 +579,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1052,17 +1055,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32:D32"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.4285714285714" style="1"/>
+    <col min="1" max="1" width="10.8571428571429" style="1"/>
     <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.4285714285714" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
@@ -1089,7 +1092,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>270875</v>
+        <v>304234</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1500,6 +1503,42 @@
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="5">
+        <v>44323</v>
+      </c>
+      <c r="B33" s="1">
+        <v>17485</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5">
+        <v>44327</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2690</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5">
+        <v>44329</v>
+      </c>
+      <c r="B35" s="1">
+        <v>13184</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
datatill 18 May 12PM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,9 +72,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -95,6 +95,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -102,56 +109,57 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,6 +180,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -179,60 +210,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,187 +265,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,6 +456,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,15 +522,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -516,23 +540,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,162 +556,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1055,12 +1055,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>304234</v>
+        <v>314234</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1539,6 +1539,17 @@
       </c>
       <c r="C35" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="5">
+        <v>44334</v>
+      </c>
+      <c r="B36" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 19May 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -94,46 +94,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,9 +118,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,6 +209,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -170,69 +224,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,187 +265,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,11 +459,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,6 +479,50 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,36 +543,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -536,40 +556,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -579,130 +579,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1060,7 +1060,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>314234</v>
+        <v>307554</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1541,15 +1541,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="5">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B36" s="1">
-        <v>10000</v>
+        <v>3320</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 5Jun 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Commission for Apr2021 Vendor ledger</t>
+  </si>
+  <si>
+    <t>GST reimbursement for April 2021</t>
   </si>
 </sst>
 </file>
@@ -72,8 +75,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -94,6 +97,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -102,9 +120,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,127 +190,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +268,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -277,13 +292,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,157 +442,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,35 +483,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -522,7 +502,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,6 +522,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -556,12 +545,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -582,131 +591,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -729,6 +738,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1055,12 +1067,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1092,7 +1104,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>307554</v>
+        <v>363194</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1301,7 +1313,7 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1409,7 +1421,7 @@
       <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1487,7 +1499,7 @@
       <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1553,6 +1565,20 @@
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="5">
+        <v>44349</v>
+      </c>
+      <c r="B37" s="1">
+        <v>55640</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till 13 June 8AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>GST reimbursement for April 2021</t>
+  </si>
+  <si>
+    <t>Commission for May 2021 Vendor ledger</t>
   </si>
 </sst>
 </file>
@@ -75,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -97,57 +100,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -159,6 +116,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -191,51 +201,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,187 +277,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,6 +468,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -479,6 +491,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,24 +551,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,31 +568,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -588,130 +591,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1067,12 +1070,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1104,7 +1107,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>363194</v>
+        <v>375513</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1579,6 +1582,20 @@
       </c>
       <c r="D37" s="8" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="5">
+        <v>44356</v>
+      </c>
+      <c r="B38" s="1">
+        <v>12319</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data till Arwal 5 July 9 AM
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jio\DailyReport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -70,20 +75,20 @@
     <t>GST reimbursement for April 2021</t>
   </si>
   <si>
-    <t>Commission for May 2021 Vendor ledger</t>
+    <t>PLI Commission for May 2021 Vendor ledger</t>
+  </si>
+  <si>
+    <t>CON03 For May20211</t>
+  </si>
+  <si>
+    <t>SIM SECURITY DEPOSIT REFUND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,152 +104,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,13 +114,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,194 +136,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -470,251 +145,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -747,66 +180,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00DD56E2"/>
+      <color rgb="FFDD56E2"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1064,27 +453,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.8571428571429" style="1"/>
-    <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.4285714285714" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.14285714285714" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1101,13 +489,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>375513</v>
+        <v>399237</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1456,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" s="5">
         <v>44301</v>
       </c>
@@ -1467,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" s="5">
         <v>44302</v>
       </c>
@@ -1534,7 +922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="5">
         <v>44327</v>
       </c>
@@ -1545,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" s="5">
         <v>44329</v>
       </c>
@@ -1598,8 +986,49 @@
         <v>18</v>
       </c>
     </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="5">
+        <v>44362</v>
+      </c>
+      <c r="B39" s="1">
+        <v>10944</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="5">
+        <v>44365</v>
+      </c>
+      <c r="B40" s="1">
+        <v>6670</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="5">
+        <v>44380</v>
+      </c>
+      <c r="B41" s="1">
+        <v>6110</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data till 11 july 8am
</commit_message>
<xml_diff>
--- a/AutoCreditAmount.xlsx
+++ b/AutoCreditAmount.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jio\DailyReport\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7965"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -82,13 +77,22 @@
   </si>
   <si>
     <t>SIM SECURITY DEPOSIT REFUND</t>
+  </si>
+  <si>
+    <t>PLI Commission for June 2021 Vendor ledger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +108,152 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,13 +262,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,8 +284,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -145,9 +479,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -180,22 +756,66 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFDD56E2"/>
+      <color rgb="00DD56E2"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -453,26 +1073,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.8571428571429" style="1"/>
+    <col min="2" max="2" width="15.5714285714286" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.4285714285714" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -489,13 +1110,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
         <f>SUM(B3:B2223)</f>
-        <v>399237</v>
+        <v>414527</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -844,7 +1465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28" s="5">
         <v>44301</v>
       </c>
@@ -855,7 +1476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3">
       <c r="A29" s="5">
         <v>44302</v>
       </c>
@@ -922,7 +1543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:3">
       <c r="A34" s="5">
         <v>44327</v>
       </c>
@@ -933,7 +1554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:3">
       <c r="A35" s="5">
         <v>44329</v>
       </c>
@@ -1028,7 +1649,22 @@
         <v>20</v>
       </c>
     </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5">
+        <v>44386</v>
+      </c>
+      <c r="B42" s="1">
+        <v>15290</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>